<commit_message>
Adding new version of modelagem spreadsheet
</commit_message>
<xml_diff>
--- a/Modelagem - MVP - Eng Dados.xlsx
+++ b/Modelagem - MVP - Eng Dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/542396adf35ec65f/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/542396adf35ec65f/PUCRJ/Pos - Ciencia de Dados e Analytics/Sprint Engenharia de Dados/MVP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{55F81600-7CB7-4562-8987-1CA0E1481EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1C8D8D4-4EC3-4256-B970-AF3CA3555ED9}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{55F81600-7CB7-4562-8987-1CA0E1481EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5008EFB6-249F-49A4-81A7-0DB9E71B6C50}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C645BDAF-C743-4BC5-AA31-5441E7DA44BB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C645BDAF-C743-4BC5-AA31-5441E7DA44BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -38,36 +38,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="113">
   <si>
-    <t>Marital Status</t>
-  </si>
-  <si>
     <t>Integer</t>
   </si>
   <si>
     <t>no</t>
   </si>
   <si>
-    <t>Application mode</t>
-  </si>
-  <si>
-    <t>Application order</t>
-  </si>
-  <si>
     <t>Application order (between 0 - first choice; and 9 last choice)</t>
   </si>
   <si>
     <t>Course</t>
   </si>
   <si>
-    <t>Daytime/evening attendance</t>
-  </si>
-  <si>
-    <t>Previous qualification</t>
-  </si>
-  <si>
-    <t>Previous qualification (grade)</t>
-  </si>
-  <si>
     <t>Continuous</t>
   </si>
   <si>
@@ -77,21 +59,6 @@
     <t>Nacionality</t>
   </si>
   <si>
-    <t>Mother's qualification</t>
-  </si>
-  <si>
-    <t>Father's qualification</t>
-  </si>
-  <si>
-    <t>Mother's occupation</t>
-  </si>
-  <si>
-    <t>Father's occupation</t>
-  </si>
-  <si>
-    <t>Admission grade</t>
-  </si>
-  <si>
     <t>Admission grade (between 0 and 200)</t>
   </si>
   <si>
@@ -101,109 +68,55 @@
     <t>1 – yes 0 – no</t>
   </si>
   <si>
-    <t>Educational special needs</t>
-  </si>
-  <si>
     <t>Debtor</t>
   </si>
   <si>
-    <t>Tuition fees up to date</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
     <t>1 – male 0 – female</t>
   </si>
   <si>
-    <t>Scholarship holder</t>
-  </si>
-  <si>
-    <t>Age at enrollment</t>
-  </si>
-  <si>
     <t>Age of studend at enrollment</t>
   </si>
   <si>
     <t>International</t>
   </si>
   <si>
-    <t>Curricular units 1st sem (credited)</t>
-  </si>
-  <si>
     <t>Number of curricular units credited in the 1st semester</t>
   </si>
   <si>
-    <t>Curricular units 1st sem (enrolled)</t>
-  </si>
-  <si>
     <t>Number of curricular units enrolled in the 1st semester</t>
   </si>
   <si>
-    <t>Curricular units 1st sem (evaluations)</t>
-  </si>
-  <si>
     <t>Number of evaluations to curricular units in the 1st semester</t>
   </si>
   <si>
-    <t>Curricular units 1st sem (approved)</t>
-  </si>
-  <si>
     <t>Number of curricular units approved in the 1st semester</t>
   </si>
   <si>
-    <t>Curricular units 1st sem (grade)</t>
-  </si>
-  <si>
     <t>Grade average in the 1st semester (between 0 and 20)</t>
   </si>
   <si>
-    <t>Curricular units 1st sem (without evaluations)</t>
-  </si>
-  <si>
     <t>Number of curricular units without evalutions in the 1st semester</t>
   </si>
   <si>
-    <t>Curricular units 2nd sem (credited)</t>
-  </si>
-  <si>
     <t>Number of curricular units credited in the 2nd semester</t>
   </si>
   <si>
-    <t>Curricular units 2nd sem (enrolled)</t>
-  </si>
-  <si>
     <t>Number of curricular units enrolled in the 2nd semester</t>
   </si>
   <si>
-    <t>Curricular units 2nd sem (evaluations)</t>
-  </si>
-  <si>
     <t>Number of evaluations to curricular units in the 2nd semester</t>
   </si>
   <si>
-    <t>Curricular units 2nd sem (approved)</t>
-  </si>
-  <si>
     <t>Number of curricular units approved in the 2nd semester</t>
   </si>
   <si>
-    <t>Curricular units 2nd sem (grade)</t>
-  </si>
-  <si>
     <t>Grade average in the 2nd semester (between 0 and 20)</t>
   </si>
   <si>
-    <t>Curricular units 2nd sem (without evaluations)</t>
-  </si>
-  <si>
-    <t>Unemployment rate</t>
-  </si>
-  <si>
     <t>Unemployment rate (%)</t>
-  </si>
-  <si>
-    <t>Inflation rate</t>
   </si>
   <si>
     <t>Inflation rate (%)</t>
@@ -587,6 +500,93 @@
 193 - Unskilled workers in extractive industry, construction, manufacturing and transport 
 194 - Meal preparation assistants 
 195 - Street vendors (except food) and street service providers</t>
+  </si>
+  <si>
+    <t>Marital_status</t>
+  </si>
+  <si>
+    <t>Application_mode</t>
+  </si>
+  <si>
+    <t>Application_order</t>
+  </si>
+  <si>
+    <t>Daytime/evening_attendance</t>
+  </si>
+  <si>
+    <t>Previous_qualification</t>
+  </si>
+  <si>
+    <t>Admission_grade</t>
+  </si>
+  <si>
+    <t>Educational_special_needs</t>
+  </si>
+  <si>
+    <t>Tuition_fees_up_to_date</t>
+  </si>
+  <si>
+    <t>Scholarship_holder</t>
+  </si>
+  <si>
+    <t>Age_at_enrollment</t>
+  </si>
+  <si>
+    <t>Unemployment_rate</t>
+  </si>
+  <si>
+    <t>Inflation_rate</t>
+  </si>
+  <si>
+    <t>Previous_qualification_grade</t>
+  </si>
+  <si>
+    <t>Mother_qualification</t>
+  </si>
+  <si>
+    <t>Father_qualification</t>
+  </si>
+  <si>
+    <t>Mother_occupation</t>
+  </si>
+  <si>
+    <t>Father_occupation</t>
+  </si>
+  <si>
+    <t>Curricular_units_1st_sem_credited</t>
+  </si>
+  <si>
+    <t>Curricular_units_1st_sem_enrolled</t>
+  </si>
+  <si>
+    <t>Curricular_units_1st_sem_evaluations</t>
+  </si>
+  <si>
+    <t>Curricular_units_1st_sem_approved</t>
+  </si>
+  <si>
+    <t>Curricular_units_1st_sem_grade</t>
+  </si>
+  <si>
+    <t>Curricular_units_1st_sem_without_evaluations</t>
+  </si>
+  <si>
+    <t>Curricular_units_2nd_sem_credited</t>
+  </si>
+  <si>
+    <t>Curricular_units_2nd_sem_enrolled</t>
+  </si>
+  <si>
+    <t>Curricular_units_2nd_sem_evaluations</t>
+  </si>
+  <si>
+    <t>Curricular_units_2nd_sem_approved</t>
+  </si>
+  <si>
+    <t>Curricular_units_2nd_sem_grade</t>
+  </si>
+  <si>
+    <t>Curricular_units_2nd_sem_without_evaluations</t>
   </si>
 </sst>
 </file>
@@ -687,36 +687,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -749,6 +719,36 @@
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -762,15 +762,19 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B9B72904-0BF8-4A35-84A7-3A2BFA6169E6}" name="Tabela1" displayName="Tabela1" ref="A1:E38" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B9B72904-0BF8-4A35-84A7-3A2BFA6169E6}" name="Tabela1" displayName="Tabela1" ref="A1:E38" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E38" xr:uid="{B9B72904-0BF8-4A35-84A7-3A2BFA6169E6}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{911BE1D9-9E2E-4578-825C-0366237E88E6}" name="Coluna" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{2D403B94-23E7-4727-AD03-940B97CA4718}" name="Tipo" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{189F3564-0D7F-40C1-B5FA-10340ED6E252}" name="Descrição" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{D6EE8EC9-157A-4DBC-A764-6FB717E1E6E3}" name="Valores" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{A9305FF0-74AC-4C4F-A415-A442D2187A2B}" name="Possui Registros Nulos/Vazios?" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{911BE1D9-9E2E-4578-825C-0366237E88E6}" name="Coluna" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{2D403B94-23E7-4727-AD03-940B97CA4718}" name="Tipo" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{189F3564-0D7F-40C1-B5FA-10340ED6E252}" name="Descrição" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{D6EE8EC9-157A-4DBC-A764-6FB717E1E6E3}" name="Valores" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{A9305FF0-74AC-4C4F-A415-A442D2187A2B}" name="Possui Registros Nulos/Vazios?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1095,7 +1099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28022E1B-41F5-4119-8A09-BBEB26DF1525}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E38" sqref="A1:E38"/>
     </sheetView>
   </sheetViews>
@@ -1110,648 +1114,648 @@
   <sheetData>
     <row r="1" spans="1:5" ht="42" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="84" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="252" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="238" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="238" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>8</v>
+        <v>88</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="294" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="406" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>14</v>
+        <v>98</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="28" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="28" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="28" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>34</v>
+        <v>103</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="28" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>38</v>
+        <v>105</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="28" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>40</v>
+        <v>106</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="28" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>42</v>
+        <v>107</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="28" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="28" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>46</v>
+        <v>109</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="28" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="28" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>52</v>
+        <v>112</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="42" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>